<commit_message>
fixed bug and add logic validate xor
</commit_message>
<xml_diff>
--- a/inputs/TestCase-ForWirteTxt.xlsx
+++ b/inputs/TestCase-ForWirteTxt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D544164A-E786-4689-B4DA-C1F02C94A47B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AF35D3-5060-4D3C-B7AA-EE96564E75DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0F3E6C9-E565-43B2-906E-B8A755B99593}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>มากกว่าหรือเท่ากับ</t>
+  </si>
+  <si>
+    <t>Variable1/Description</t>
+  </si>
+  <si>
+    <t>Variable2/Description</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -608,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>

</xml_diff>